<commit_message>
Fix column formating in excel template
Related Work Items: #6168
</commit_message>
<xml_diff>
--- a/web/Content/Files/consignment_list_format_template.xlsx
+++ b/web/Content/Files/consignment_list_format_template.xlsx
@@ -725,7 +725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1090,33 +1090,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -1236,8 +1236,6 @@
       <c r="G2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
@@ -1253,7 +1251,6 @@
       <c r="N2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1364,8 +1361,6 @@
       <c r="T3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
       <c r="W3" s="1" t="s">
         <v>47</v>
       </c>

</xml_diff>